<commit_message>
Update on RTS 15/08/2025
</commit_message>
<xml_diff>
--- a/testNadz/2.Web/AutoReg_FBG2.0_Happy_Flow_E2E_Web.xlsx
+++ b/testNadz/2.Web/AutoReg_FBG2.0_Happy_Flow_E2E_Web.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -502,9 +502,69 @@
         <v>N/A</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>WEB_AdminLogin</v>
+      </c>
+      <c r="B6" t="str">
+        <v>TC001A</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Web_Admin_FB_Approve_SupplierManagement_CompanyDetails_HappyFlow</v>
+      </c>
+      <c r="D6" t="str">
+        <v>8/15/2025, 12:23:52 PM</v>
+      </c>
+      <c r="E6" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="F6" t="str">
+        <v>/Users/adlanelias/Documents/Nadz/VSCode/FarmbytesNadz-1/testNadz/2.Web/screenshots/web_FB_approve_supplier_management_CompanyInfo/step1_error.png</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>WEB_AdminLogin</v>
+      </c>
+      <c r="B7" t="str">
+        <v>TC001A</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Web_Admin_FB_Approve_SupplierManagement_CompanyDetails_HappyFlow</v>
+      </c>
+      <c r="D7" t="str">
+        <v>8/15/2025, 12:25:03 PM</v>
+      </c>
+      <c r="E7" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Screenshot failed</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>WEB_AdminLogin</v>
+      </c>
+      <c r="B8" t="str">
+        <v>TC005B</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Web_Admin_Email_RTS_Assign_Logistic</v>
+      </c>
+      <c r="D8" t="str">
+        <v>8/15/2025, 12:46:47 PM</v>
+      </c>
+      <c r="E8" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Screenshot failed</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
RTS PurchaseOrder 20/08/2025 v12
</commit_message>
<xml_diff>
--- a/testNadz/2.Web/AutoReg_FBG2.0_Happy_Flow_E2E_Web.xlsx
+++ b/testNadz/2.Web/AutoReg_FBG2.0_Happy_Flow_E2E_Web.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1802,9 +1802,29 @@
         <v>/Users/adlanelias/Documents/Nadz/VSCode/FarmbytesNadz-1/testNadz/2.Web/screenshots/web_Email_RTS_BeginGrading/step14_approve_signoff_grading.png</v>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>WEB_AdminLogin</v>
+      </c>
+      <c r="B71" t="str">
+        <v>TC005D</v>
+      </c>
+      <c r="C71" t="str">
+        <v>Web_Admin_Email_RTS_BeginGrading</v>
+      </c>
+      <c r="D71" t="str">
+        <v>8/20/2025, 6:53:55 PM</v>
+      </c>
+      <c r="E71" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="F71" t="str">
+        <v>Screenshot failed</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F70"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F71"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated on 03/09/2025 v2
</commit_message>
<xml_diff>
--- a/testNadz/2.Web/AutoReg_FBG2.0_Happy_Flow_E2E_Web.xlsx
+++ b/testNadz/2.Web/AutoReg_FBG2.0_Happy_Flow_E2E_Web.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F273"/>
+  <dimension ref="A1:F274"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -5862,9 +5862,29 @@
         <v>Screenshot failed</v>
       </c>
     </row>
+    <row r="274">
+      <c r="A274" t="str">
+        <v>WEB_AdminLogin</v>
+      </c>
+      <c r="B274" t="str">
+        <v>TC005A</v>
+      </c>
+      <c r="C274" t="str">
+        <v>Web_Admin_Email_RTS_Approve_Quote_DriverCollect</v>
+      </c>
+      <c r="D274" t="str">
+        <v>9/3/2025, 2:34:10 PM</v>
+      </c>
+      <c r="E274" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="F274" t="str">
+        <v>/Users/adlanelias/Documents/Nadz/VSCode/FarmbytesNadz-1/testNadz/2.Web/screenshots/web_Email_RTS_Approve_Quote_DriverCollect/step8_quotation_approved.png</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F273"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F274"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>